<commit_message>
cleaning up metabolomics util funtions
</commit_message>
<xml_diff>
--- a/metabolomics_analysis/processed_data/spent_media_pca_data.xlsx
+++ b/metabolomics_analysis/processed_data/spent_media_pca_data.xlsx
@@ -462,16 +462,16 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-23.75530573991148</v>
+        <v>-23.7553057399115</v>
       </c>
       <c r="C2" t="n">
-        <v>-2.747022348025979</v>
+        <v>-2.747022348026007</v>
       </c>
       <c r="D2" t="n">
-        <v>16.79049191890008</v>
+        <v>16.79049191890009</v>
       </c>
       <c r="E2" t="n">
-        <v>-2.730595491294519</v>
+        <v>-2.730595491294502</v>
       </c>
     </row>
     <row r="3">
@@ -481,16 +481,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-21.32040961172909</v>
+        <v>-21.3204096117291</v>
       </c>
       <c r="C3" t="n">
-        <v>-1.552455659040826</v>
+        <v>-1.552455659040844</v>
       </c>
       <c r="D3" t="n">
-        <v>19.31914670088395</v>
+        <v>19.31914670088397</v>
       </c>
       <c r="E3" t="n">
-        <v>3.419550768428692</v>
+        <v>3.419550768428719</v>
       </c>
     </row>
     <row r="4">
@@ -500,16 +500,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-24.14681937886425</v>
+        <v>-24.14681937886427</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.7353431566746569</v>
+        <v>-0.7353431566746778</v>
       </c>
       <c r="D4" t="n">
-        <v>14.83433347702452</v>
+        <v>14.83433347702454</v>
       </c>
       <c r="E4" t="n">
-        <v>-2.332512537181795</v>
+        <v>-2.332512537181791</v>
       </c>
     </row>
     <row r="5">
@@ -519,16 +519,16 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-8.519638425765876</v>
+        <v>-8.519638425765878</v>
       </c>
       <c r="C5" t="n">
-        <v>-21.39506130043912</v>
+        <v>-21.39506130043913</v>
       </c>
       <c r="D5" t="n">
-        <v>-10.23278226362014</v>
+        <v>-10.23278226362016</v>
       </c>
       <c r="E5" t="n">
-        <v>2.948777486331835</v>
+        <v>2.94877748633183</v>
       </c>
     </row>
     <row r="6">
@@ -541,13 +541,13 @@
         <v>-12.01619743888462</v>
       </c>
       <c r="C6" t="n">
-        <v>-22.81184356343839</v>
+        <v>-22.8118435634384</v>
       </c>
       <c r="D6" t="n">
-        <v>-13.31435700989718</v>
+        <v>-13.3143570098972</v>
       </c>
       <c r="E6" t="n">
-        <v>0.008099017127514686</v>
+        <v>0.008099017127518392</v>
       </c>
     </row>
     <row r="7">
@@ -557,16 +557,16 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-9.091583701216129</v>
+        <v>-9.091583701216132</v>
       </c>
       <c r="C7" t="n">
         <v>-19.43931142253502</v>
       </c>
       <c r="D7" t="n">
-        <v>-6.422217902891713</v>
+        <v>-6.422217902891732</v>
       </c>
       <c r="E7" t="n">
-        <v>7.092254042592723</v>
+        <v>7.092254042592721</v>
       </c>
     </row>
     <row r="8">
@@ -576,16 +576,16 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-18.20805696000487</v>
+        <v>-18.20805696000488</v>
       </c>
       <c r="C8" t="n">
-        <v>23.65227488235066</v>
+        <v>23.6522748823507</v>
       </c>
       <c r="D8" t="n">
-        <v>-11.56380746719227</v>
+        <v>-11.56380746719226</v>
       </c>
       <c r="E8" t="n">
-        <v>0.4324392164856478</v>
+        <v>0.4324392164856246</v>
       </c>
     </row>
     <row r="9">
@@ -595,16 +595,16 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-19.76975158045608</v>
+        <v>-19.76975158045609</v>
       </c>
       <c r="C9" t="n">
-        <v>15.02925707634848</v>
+        <v>15.0292570763485</v>
       </c>
       <c r="D9" t="n">
-        <v>-7.060786030201702</v>
+        <v>-7.060786030201677</v>
       </c>
       <c r="E9" t="n">
-        <v>-14.75322444489173</v>
+        <v>-14.75322444489174</v>
       </c>
     </row>
     <row r="10">
@@ -614,16 +614,16 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-15.47060744100156</v>
+        <v>-15.47060744100157</v>
       </c>
       <c r="C10" t="n">
-        <v>23.42896378182417</v>
+        <v>23.42896378182421</v>
       </c>
       <c r="D10" t="n">
         <v>-9.209905775189421</v>
       </c>
       <c r="E10" t="n">
-        <v>8.775214946078648</v>
+        <v>8.775214946078634</v>
       </c>
     </row>
     <row r="11">
@@ -633,16 +633,16 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>46.20490571345204</v>
+        <v>46.20490571345206</v>
       </c>
       <c r="C11" t="n">
-        <v>0.6320184367918672</v>
+        <v>0.6320184367918684</v>
       </c>
       <c r="D11" t="n">
-        <v>-1.106626292784662</v>
+        <v>-1.106626292784664</v>
       </c>
       <c r="E11" t="n">
-        <v>-8.214756245398446</v>
+        <v>-8.214756245398455</v>
       </c>
     </row>
     <row r="12">
@@ -652,13 +652,13 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>53.35112947825327</v>
+        <v>53.35112947825331</v>
       </c>
       <c r="C12" t="n">
-        <v>-2.303671467059281</v>
+        <v>-2.303671467059289</v>
       </c>
       <c r="D12" t="n">
-        <v>2.847568830084668</v>
+        <v>2.847568830084677</v>
       </c>
       <c r="E12" t="n">
         <v>-15.57004937123718</v>
@@ -671,16 +671,16 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>52.74233508612864</v>
+        <v>52.74233508612866</v>
       </c>
       <c r="C13" t="n">
-        <v>8.242194739898084</v>
+        <v>8.242194739898093</v>
       </c>
       <c r="D13" t="n">
-        <v>5.118941814883859</v>
+        <v>5.11894181488383</v>
       </c>
       <c r="E13" t="n">
-        <v>20.9248026129586</v>
+        <v>20.92480261295862</v>
       </c>
     </row>
   </sheetData>

</xml_diff>